<commit_message>
Runmode yes for all testcases
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/LogixalQABox2/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/LogixalQABox2/MasterExecutor_Sanity.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Master_executors\LogixalQABox2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AEF1F0-EECB-4301-A574-578EC4ECD1C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterExecutor" sheetId="10" r:id="rId1"/>
@@ -248,13 +254,13 @@
     <t>TC34_Verify_Contactus_form_submission</t>
   </si>
   <si>
-    <t>NO</t>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -397,16 +403,19 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 3" xfId="4"/>
-    <cellStyle name="Normal 5" xfId="3"/>
-    <cellStyle name="Normal 6" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 6" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -740,11 +749,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>